<commit_message>
added pin compatible part
</commit_message>
<xml_diff>
--- a/Hardware/K02_128_Clock2/Fab_v1.5/BOM_PCBWay_K02_128_Clock2_V1.5.xlsx
+++ b/Hardware/K02_128_Clock2/Fab_v1.5/BOM_PCBWay_K02_128_Clock2_V1.5.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0210A-C1BC-4D67-AF79-76B0009B6FE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C746DEE7-8829-4E36-9255-FE3E686A162A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3840" yWindow="-15615" windowWidth="26565" windowHeight="11685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1605" yWindow="-17640" windowWidth="25320" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="155">
   <si>
     <t>Item #</t>
   </si>
@@ -479,9 +479,6 @@
     <t>K02FN128VFM10, 128 KB Flash, 16 KB RAM, 32QFN</t>
   </si>
   <si>
-    <t xml:space="preserve">Mouser: 841-MK02FN128VFM10 </t>
-  </si>
-  <si>
     <t>Mouser: 453-DIO7003LAST5</t>
   </si>
   <si>
@@ -558,13 +555,19 @@
   </si>
   <si>
     <t>B2B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t>Mouser: 841-MK02FN128VFM10</t>
+  </si>
+  <si>
+    <t>MK02FN64VFM10 (pin compatible, but less FLASH)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,6 +634,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -691,7 +700,7 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -724,12 +733,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -777,6 +780,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1168,8 +1180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1188,25 +1200,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="D2" s="12" t="s">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="D2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1241,13 +1253,13 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="18">
+      <c r="A7" s="16">
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1256,7 +1268,7 @@
       <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="19" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -1268,48 +1280,48 @@
       <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="21" t="s">
+      <c r="J7" s="19" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="18">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>1</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="25" t="s">
         <v>135</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>136</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="21" t="s">
-        <v>132</v>
+      <c r="J8" s="19" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="18">
+      <c r="A9" s="16">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1318,7 +1330,7 @@
       <c r="E9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="19" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -1330,18 +1342,18 @@
       <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="21" t="s">
+      <c r="J9" s="19" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="18">
+      <c r="A10" s="16">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1350,7 +1362,7 @@
       <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="19" t="s">
         <v>54</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -1362,18 +1374,18 @@
       <c r="I10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="19" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="18">
+      <c r="A11" s="16">
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1382,7 +1394,7 @@
       <c r="E11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="19" t="s">
         <v>59</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -1394,28 +1406,28 @@
       <c r="I11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="21" t="s">
+      <c r="J11" s="19" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="18">
+      <c r="A12" s="16">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="16">
         <v>2</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="F12" s="26" t="s">
         <v>138</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>139</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>13</v>
@@ -1426,18 +1438,18 @@
       <c r="I12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="21" t="s">
-        <v>140</v>
+      <c r="J12" s="19" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="18">
+      <c r="A13" s="16">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1446,7 +1458,7 @@
       <c r="E13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="27" t="s">
         <v>76</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -1455,31 +1467,31 @@
       <c r="H13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="22"/>
+      <c r="I13" s="20"/>
       <c r="J13" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="10" customFormat="1">
-      <c r="A14" s="19">
+      <c r="A14" s="17">
         <v>8</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="17">
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="F14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="9" t="s">
@@ -1488,30 +1500,30 @@
       <c r="I14" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="23" t="s">
-        <v>150</v>
+      <c r="J14" s="21" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1">
-      <c r="A15" s="19">
+      <c r="A15" s="17">
         <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="17">
         <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="9" t="s">
@@ -1520,30 +1532,30 @@
       <c r="I15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J15" s="23" t="s">
-        <v>148</v>
+      <c r="J15" s="21" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="10" customFormat="1">
-      <c r="A16" s="19">
+      <c r="A16" s="17">
         <v>10</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="17">
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F16" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H16" s="9" t="s">
@@ -1552,18 +1564,18 @@
       <c r="I16" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J16" s="23" t="s">
-        <v>149</v>
+      <c r="J16" s="21" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="17">
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -1584,18 +1596,18 @@
       <c r="I17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="21" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1">
-      <c r="A18" s="19">
+      <c r="A18" s="17">
         <v>12</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="19">
+      <c r="C18" s="17">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -1616,18 +1628,18 @@
       <c r="I18" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="21" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="8" customFormat="1">
-      <c r="A19" s="20">
+      <c r="A19" s="18">
         <v>13</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="18">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1639,27 +1651,27 @@
       <c r="F19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H19" s="13" t="s">
         <v>3</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="21" t="s">
+      <c r="J19" s="19" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="8" customFormat="1">
-      <c r="A20" s="20">
+      <c r="A20" s="18">
         <v>14</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1671,27 +1683,27 @@
       <c r="F20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="13" t="s">
         <v>3</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="8" customFormat="1">
-      <c r="A21" s="20">
+      <c r="A21" s="18">
         <v>15</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="18">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1703,27 +1715,27 @@
       <c r="F21" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="13" t="s">
         <v>3</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="22" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="8" customFormat="1">
-      <c r="A22" s="20">
+      <c r="A22" s="18">
         <v>16</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="18">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -1735,27 +1747,27 @@
       <c r="F22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="13" t="s">
         <v>3</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J22" s="24" t="s">
+      <c r="J22" s="22" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="8" customFormat="1">
-      <c r="A23" s="20">
+      <c r="A23" s="18">
         <v>17</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="18">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -1764,28 +1776,28 @@
       <c r="E23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="25"/>
+      <c r="I23" s="23"/>
       <c r="J23" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1">
-      <c r="A24" s="19">
+      <c r="A24" s="17">
         <v>18</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="17">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1797,7 +1809,7 @@
       <c r="F24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="9" t="s">
@@ -1806,18 +1818,18 @@
       <c r="I24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="21" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="8" customFormat="1">
-      <c r="A25" s="20">
+      <c r="A25" s="18">
         <v>19</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="18">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -1826,58 +1838,58 @@
       <c r="E25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="G25" s="16" t="s">
+      <c r="F25" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="25"/>
-      <c r="J25" s="21" t="s">
+      <c r="I25" s="23"/>
+      <c r="J25" s="19" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="8" customFormat="1">
-      <c r="A26" s="20">
+      <c r="A26" s="18">
         <v>20</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="18">
         <v>1</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D26" s="19" t="s">
         <v>84</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="29" t="s">
-        <v>145</v>
-      </c>
-      <c r="G26" s="22" t="s">
+      <c r="F26" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G26" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="H26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I26" s="25"/>
-      <c r="J26" s="21" t="s">
+      <c r="I26" s="23"/>
+      <c r="J26" s="19" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="8" customFormat="1">
-      <c r="A27" s="20">
+      <c r="A27" s="18">
         <v>21</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="18">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
@@ -1889,55 +1901,57 @@
       <c r="F27" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="30"/>
-      <c r="J27" s="24" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="8" customFormat="1" ht="15">
-      <c r="A28" s="20">
+      <c r="I27" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="8" customFormat="1">
+      <c r="A28" s="18">
         <v>22</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="18">
         <v>1</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="F28" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="30"/>
-      <c r="J28" s="24" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="29" spans="1:10" s="8" customFormat="1">
-      <c r="A29" s="20">
+      <c r="A29" s="18">
         <v>23</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="18">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
@@ -1946,58 +1960,58 @@
       <c r="E29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="15" t="s">
         <v>97</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="30"/>
-      <c r="J29" s="24" t="s">
-        <v>131</v>
+      <c r="I29" s="28"/>
+      <c r="J29" s="22" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="8" customFormat="1">
-      <c r="A30" s="20">
+      <c r="A30" s="18">
         <v>24</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="18">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="15" t="s">
         <v>125</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I30" s="30"/>
-      <c r="J30" s="24" t="s">
-        <v>128</v>
+      <c r="I30" s="28"/>
+      <c r="J30" s="22" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="8" customFormat="1">
-      <c r="A31" s="20">
+      <c r="A31" s="18">
         <v>25</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="18">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2006,28 +2020,28 @@
       <c r="E31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="15" t="s">
         <v>122</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="21" t="s">
+      <c r="I31" s="13"/>
+      <c r="J31" s="19" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="8" customFormat="1">
-      <c r="A32" s="20">
+      <c r="A32" s="18">
         <v>26</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="18">
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -2036,21 +2050,32 @@
       <c r="E32" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="29" t="s">
+      <c r="F32" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="15" t="s">
         <v>87</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="24" t="s">
+      <c r="I32" s="13"/>
+      <c r="J32" s="22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="33" spans="1:10">
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>